<commit_message>
upto data provider -3
</commit_message>
<xml_diff>
--- a/Data/data1.xlsx
+++ b/Data/data1.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="10755" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19095" windowHeight="10755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Add Customer" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>admin</t>
   </si>
@@ -58,14 +59,40 @@
   </si>
   <si>
     <t>pune2</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>expected url</t>
+  </si>
+  <si>
+    <t>http://stock.scriptinglogic.net/index.php?msg=Wrong%20Username%20or%20Password&amp;type=error</t>
+  </si>
+  <si>
+    <t>http://stock.scriptinglogic.net/dashboard.php</t>
+  </si>
+  <si>
+    <t>expected Page title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,9 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +423,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -440,23 +470,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -464,10 +494,10 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>67676</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>676767</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -478,10 +508,10 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>67676</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>676767</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -496,12 +526,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4:C5" r:id="rId2" display="http://stock.scriptinglogic.net/index.php?msg=Wrong%20Username%20or%20Password&amp;type=error"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>